<commit_message>
Updated data manager to now support HTC and CECAP datasets Added tool for closing Excel running in the background
</commit_message>
<xml_diff>
--- a/WpfApplication1/staticdata/IndicatorDefinitions.xlsx
+++ b/WpfApplication1/staticdata/IndicatorDefinitions.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\github\xl-template-reader\template-reader\template-reader\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\github\ZambiaDataManager\WpfApplication1\staticdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IndicatorDefinitions" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="progarea">Sheet1!$F$2:$H$9</definedName>
-    <definedName name="programareas">Sheet1!$B$2:$D$9</definedName>
+    <definedName name="progarea">Sheet1!$F$2:$H$11</definedName>
+    <definedName name="programareas">Sheet1!$B$2:$D$11</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="415">
   <si>
     <t>ProgramArea</t>
   </si>
@@ -1071,13 +1072,275 @@
   </si>
   <si>
     <t>IndicatorId</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>CECAP</t>
+  </si>
+  <si>
+    <t>CECAP 1</t>
+  </si>
+  <si>
+    <t>Number of clients who received a VIA screening (Total)</t>
+  </si>
+  <si>
+    <t>CECAP 2</t>
+  </si>
+  <si>
+    <t>Number of  new women screened using VIA (New)</t>
+  </si>
+  <si>
+    <t>CECAP 3</t>
+  </si>
+  <si>
+    <t>Number of clients who had HIV test done and received results (during screening) this month</t>
+  </si>
+  <si>
+    <t>CECAP 4</t>
+  </si>
+  <si>
+    <t>Number of New women screened using VIA and tested for HIV</t>
+  </si>
+  <si>
+    <t>CECAP 5</t>
+  </si>
+  <si>
+    <t>Total Number of women screen for VIA with Positive HIV test result.</t>
+  </si>
+  <si>
+    <t>CECAP 6</t>
+  </si>
+  <si>
+    <t>Number of clients with NEGATIVE VIA result</t>
+  </si>
+  <si>
+    <t>CECAP 7</t>
+  </si>
+  <si>
+    <t>Number of clients with POSITIVE VIA result</t>
+  </si>
+  <si>
+    <t>CECAP 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of clients with VIA today AND cryotherapy performed today. (SVA) </t>
+  </si>
+  <si>
+    <t>CECAP 9</t>
+  </si>
+  <si>
+    <t>Number of clients with previously postponed cryotherapy performed today</t>
+  </si>
+  <si>
+    <t>CECAP 10</t>
+  </si>
+  <si>
+    <t>Number of clients with VIA today AND cryotherapy postponed</t>
+  </si>
+  <si>
+    <t>CECAP 11</t>
+  </si>
+  <si>
+    <t>Number of clients referred for large lesions</t>
+  </si>
+  <si>
+    <t>CECAP 12</t>
+  </si>
+  <si>
+    <t>Number of clients with suspected cancer</t>
+  </si>
+  <si>
+    <t>CECAP 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of clients with a post-treatment complication </t>
+  </si>
+  <si>
+    <t>CECAP 14</t>
+  </si>
+  <si>
+    <t>Number new women treated with cryotherapy</t>
+  </si>
+  <si>
+    <t>CECAP 15</t>
+  </si>
+  <si>
+    <t>Total number of unique clients seen this month</t>
+  </si>
+  <si>
+    <t>CT1</t>
+  </si>
+  <si>
+    <t>Total No. of clients who were counselled and tested for HIV and received their test results  at the facility Including PITC this month.</t>
+  </si>
+  <si>
+    <t>CT1a.1</t>
+  </si>
+  <si>
+    <t>CT1b</t>
+  </si>
+  <si>
+    <t>CT1b.1</t>
+  </si>
+  <si>
+    <t>Number of clients who tested as couple and collected test results at this facility this month.</t>
+  </si>
+  <si>
+    <t>CT1c</t>
+  </si>
+  <si>
+    <t>Numbner of HIV DISCONDANT couples who received test results. (Count Females only).</t>
+  </si>
+  <si>
+    <t>CT1c.1</t>
+  </si>
+  <si>
+    <t>Number of clients who were re-tested for HIV and received there results</t>
+  </si>
+  <si>
+    <t>CT1d</t>
+  </si>
+  <si>
+    <t>Number of clients who re-tested and tested positive for HIV.</t>
+  </si>
+  <si>
+    <t>CT.e</t>
+  </si>
+  <si>
+    <t>CT.e.1</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through PMTCT</t>
+  </si>
+  <si>
+    <t>CT.e.2</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through TB</t>
+  </si>
+  <si>
+    <t>CT.e.3</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through STI</t>
+  </si>
+  <si>
+    <t>CT.e.4</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through FP</t>
+  </si>
+  <si>
+    <t>CT.e.5</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through CECAP</t>
+  </si>
+  <si>
+    <t>CT.e.6</t>
+  </si>
+  <si>
+    <t>Number of clients who tested for HIV through VMMC</t>
+  </si>
+  <si>
+    <t>CT.e.7</t>
+  </si>
+  <si>
+    <t>Number of Clients who tested positive from PITC</t>
+  </si>
+  <si>
+    <t>CT.f</t>
+  </si>
+  <si>
+    <t>Total number of clients referred for Pre ART Care Services this Months</t>
+  </si>
+  <si>
+    <t>No. of clients who received counseling and testing (CT) services for HIV and received their test results this month</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number of </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> clients who </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tested  HIV positive for HIV and collected test results.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Numbner of clients who Tested for HIV through PITC </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Total of PMTCT,STI,TB,MC,CECAP,FP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Number of all clients who tested  HIV positive for HIV and collected test results.</t>
+  </si>
+  <si>
+    <t>Numbner of clients who Tested for HIV through PITC (Total of PMTCT,STI,TB,MC,CECAP,FP)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1212,8 +1475,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,8 +1684,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1509,6 +1806,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1554,8 +1916,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1877,21 +2264,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G169" sqref="G169:G199"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="83.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +2301,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1936,7 +2326,7 @@
         <v>select 1 IndicatorSerial , 'STI1' IndicatorId, 'Number of  clients diagnosed, treated and counselled  for STI (index plus partners)' IndicatorDescription, 1 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1961,7 +2351,7 @@
         <v>select 2 IndicatorSerial , 'STI2' IndicatorId, 'Number of STI partners treated' IndicatorDescription, 2 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1986,7 +2376,7 @@
         <v>select 3 IndicatorSerial , 'STI3' IndicatorId, 'Number of clients referred for HIV Counseling and Testing' IndicatorDescription, 3 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +2401,7 @@
         <v>select 4 IndicatorSerial , 'STI4' IndicatorId, 'Number of clients tested for HIV' IndicatorDescription, 4 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2036,7 +2426,7 @@
         <v>select 5 IndicatorSerial , 'STI4a' IndicatorId, 'Number of clients tested HIV positive' IndicatorDescription, 5 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2061,7 +2451,7 @@
         <v>select 6 IndicatorSerial , 'STI5' IndicatorId, 'Number of clients referred for HIV care services' IndicatorDescription, 6 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2086,7 +2476,7 @@
         <v>select 7 IndicatorSerial , 'STI6' IndicatorId, 'Number of partner notification slips issued' IndicatorDescription, 7 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2501,7 @@
         <v>select 8 IndicatorSerial , 'STI7' IndicatorId, 'Number of partner notification slips received(of those issued by your facility)' IndicatorDescription, 8 zPosition , 4 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2136,7 +2526,7 @@
         <v>select 9 IndicatorSerial , 'TB1' IndicatorId, 'Number of presumptive TB patients  with sputum sent' IndicatorDescription, 9 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2161,7 +2551,7 @@
         <v>select 10 IndicatorSerial , 'TB2' IndicatorId, 'Number of registered new and relapse TB cases this month' IndicatorDescription, 10 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2186,7 +2576,7 @@
         <v>select 11 IndicatorSerial , 'TB3' IndicatorId, 'Number of TB patients receiving Counselling and Testing services and had results recorded in the TB Register' IndicatorDescription, 11 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2211,7 +2601,7 @@
         <v>select 12 IndicatorSerial , 'TB4' IndicatorId, 'Number of registered new and relapse TB patients with documented HIV-Negative status during TB treatment this month' IndicatorDescription, 12 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2236,7 +2626,7 @@
         <v>select 13 IndicatorSerial , 'TB5_1' IndicatorId, 'Number of registered new and relapse TB patients with documented HIV-positive status during TB treatment this month- Newly diagnozed' IndicatorDescription, 13 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2261,7 +2651,7 @@
         <v>select 14 IndicatorSerial , 'TB5_2' IndicatorId, 'Number of registered new and relapse TB patients with documented HIV-positive status during TB treatment this month- Known Positive at entry' IndicatorDescription, 14 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2286,7 +2676,7 @@
         <v>select 15 IndicatorSerial , 'TB5_3' IndicatorId, 'Total number of registered new and relapse TB patients with documented HIV-positive status who are on ART during TB treatment during this month' IndicatorDescription, 15 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2311,7 +2701,7 @@
         <v>select 16 IndicatorSerial , 'TB5a' IndicatorId, 'Number of registered new and relapse TB patients with documented HIV-positive status who are on ART this month' IndicatorDescription, 16 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2336,7 +2726,7 @@
         <v>select 17 IndicatorSerial , 'TB5b' IndicatorId, 'ART initiation less than 8 weeks of start of TB treatment' IndicatorDescription, 17 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2361,7 +2751,7 @@
         <v>select 18 IndicatorSerial , 'TB5c' IndicatorId, 'ART initiation greater than 8 weeks of start of TB treatment' IndicatorDescription, 18 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2386,7 +2776,7 @@
         <v>select 19 IndicatorSerial , 'TB6' IndicatorId, 'Number of TB patients refered for HIV care  services' IndicatorDescription, 19 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2411,7 +2801,7 @@
         <v>select 20 IndicatorSerial , 'TB7' IndicatorId, 'Number of PLHIV newly enrolled in HIV clinical care who started IPT and receive at least one dose, during this month' IndicatorDescription, 20 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2436,7 +2826,7 @@
         <v>select 21 IndicatorSerial , 'TB8' IndicatorId, 'Number of patients current on TB treatment' IndicatorDescription, 21 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2461,7 +2851,7 @@
         <v>select 22 IndicatorSerial , 'TB9' IndicatorId, 'Number of TB patients who had  follow up sputum smear at 2 months done in the reporting month' IndicatorDescription, 22 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2486,7 +2876,7 @@
         <v>select 23 IndicatorSerial , 'TB10' IndicatorId, 'Number of TB patients expected to have final outcome this month' IndicatorDescription, 23 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2511,7 +2901,7 @@
         <v>select 24 IndicatorSerial , 'TB11' IndicatorId, 'Number of patients who completed TB treatment this month' IndicatorDescription, 24 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2536,7 +2926,7 @@
         <v>select 25 IndicatorSerial , 'TB11_2' IndicatorId, 'Number of TB patients cured' IndicatorDescription, 25 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2561,7 +2951,7 @@
         <v>select 26 IndicatorSerial , 'TB12' IndicatorId, 'Number of TB patients successfully treated' IndicatorDescription, 26 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2586,7 +2976,7 @@
         <v>select 27 IndicatorSerial , 'TB13' IndicatorId, 'Number of TB Patients who died' IndicatorDescription, 27 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2611,7 +3001,7 @@
         <v>select 28 IndicatorSerial , 'TB14' IndicatorId, 'Number of TB patients who transferred out' IndicatorDescription, 28 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2636,7 +3026,7 @@
         <v>select 29 IndicatorSerial , 'TB15' IndicatorId, 'Number of TB patients  transferred in' IndicatorDescription, 29 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2661,7 +3051,7 @@
         <v>select 30 IndicatorSerial , 'TB16' IndicatorId, 'Number of TB patients who defaulted' IndicatorDescription, 30 zPosition , 5 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2686,7 +3076,7 @@
         <v>select 31 IndicatorSerial , 'ART1' IndicatorId, 'Number of adults and children receiving antiretroviral therapy (ART) [current]' IndicatorDescription, 31 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2711,7 +3101,7 @@
         <v>select 32 IndicatorSerial , 'ART2' IndicatorId, 'Number of adults and children newly enrolled on antiretroviral therapy (ART) (including pregnant  women on option B+)' IndicatorDescription, 32 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2736,7 +3126,7 @@
         <v>select 33 IndicatorSerial , 'ART2a' IndicatorId, 'Number of pregnant women newly initiating ART (option B+)' IndicatorDescription, 33 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2761,7 +3151,7 @@
         <v>select 34 IndicatorSerial , 'ART3' IndicatorId, 'No of NEW clients initiated on ART due to HIV DISCORDANT STATUS' IndicatorDescription, 34 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2786,7 +3176,7 @@
         <v>select 35 IndicatorSerial , 'ART4' IndicatorId, 'Number of individuals who ever received antiretroviral therapy (TOTAL CLIENTS)' IndicatorDescription, 35 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2811,7 +3201,7 @@
         <v>select 36 IndicatorSerial , 'ART5' IndicatorId, 'No. of pregnant women who have EVER received antiretroviral therapy (TOTAL CLIENTS)' IndicatorDescription, 36 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2836,7 +3226,7 @@
         <v>select 37 IndicatorSerial , 'ART6a' IndicatorId, 'Number  of ART clients who are transferred in from another site' IndicatorDescription, 37 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2861,7 +3251,7 @@
         <v>select 38 IndicatorSerial , 'ART6b' IndicatorId, 'Number of ART clients who stopped treatment due to loss to follow-up' IndicatorDescription, 38 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -2886,7 +3276,7 @@
         <v>select 39 IndicatorSerial , 'ART6c' IndicatorId, 'Number of ART clients Lost â€“to-follow up (LTFU) returned to the clinic.' IndicatorDescription, 39 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -2911,7 +3301,7 @@
         <v>select 40 IndicatorSerial , 'ART6d' IndicatorId, 'Number of ART clients who stopped treatment due to death' IndicatorDescription, 40 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2936,7 +3326,7 @@
         <v>select 41 IndicatorSerial , 'ART6e' IndicatorId, 'Number of ART clients who restarted treatment' IndicatorDescription, 41 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -2961,7 +3351,7 @@
         <v>select 42 IndicatorSerial , 'ART6f' IndicatorId, 'Number of ART clients transferred out to another facility' IndicatorDescription, 42 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -2986,7 +3376,7 @@
         <v>select 43 IndicatorSerial , 'ART7a' IndicatorId, 'Number of adults and children initiated on ART 12 months ago (cohort month) including pregnant women on Option B+' IndicatorDescription, 43 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -3011,7 +3401,7 @@
         <v>select 44 IndicatorSerial , 'ART7b' IndicatorId, 'Number of adults and children known to be alive and on treatment 12 months after initiation of antiretroviral therapy' IndicatorDescription, 44 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -3036,7 +3426,7 @@
         <v>select 45 IndicatorSerial , 'ART8' IndicatorId, 'Number of clients on ART have bio-chemical investigations done this month' IndicatorDescription, 45 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -3061,7 +3451,7 @@
         <v>select 46 IndicatorSerial , 'ART9' IndicatorId, 'Number of adult and pediatric ART patients who had there sample collected and sent for viral load test this month.' IndicatorDescription, 46 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -3086,7 +3476,7 @@
         <v>select 47 IndicatorSerial , 'ART10a' IndicatorId, 'Number of adult and pediatric ART patients with a viral load result documented in the patient medical record this month.' IndicatorDescription, 47 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -3111,7 +3501,7 @@
         <v>select 48 IndicatorSerial , 'ART10b' IndicatorId, 'Number of viral load tests from adult and pediatric ART patients conducted this month with a viral load &lt;1,000 copies/ml' IndicatorDescription, 48 zPosition , 1 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -3136,7 +3526,7 @@
         <v>select 49 IndicatorSerial , 'PMTCT1' IndicatorId, 'No. of New ANC Attendances' IndicatorDescription, 49 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -3161,7 +3551,7 @@
         <v>select 50 IndicatorSerial , 'PMTCT1a' IndicatorId, 'Number of pregnant women with known (positive) HIV infection attending ANC (known positives at entry)' IndicatorDescription, 50 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -3186,7 +3576,7 @@
         <v>select 51 IndicatorSerial , 'PMTCT2' IndicatorId, 'Number of pregnant women receiving PMTCT services (counseled, tested and received test results at this site during ANC and L&amp;D  the reporting period)' IndicatorDescription, 51 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -3211,7 +3601,7 @@
         <v>select 52 IndicatorSerial , 'PMTCT3' IndicatorId, 'Number of ALL pregnant women who tested positive for HIV' IndicatorDescription, 52 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -3236,7 +3626,7 @@
         <v>select 53 IndicatorSerial , 'PMTCT4' IndicatorId, 'Number of ALL pregnant women who tested positive for HIV and collected the test results' IndicatorDescription, 53 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -3261,7 +3651,7 @@
         <v>select 54 IndicatorSerial , 'PMTCT2a' IndicatorId, 'No. of pregnant women receiving PMTCT services with partner' IndicatorDescription, 54 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -3286,7 +3676,7 @@
         <v>select 55 IndicatorSerial , 'PMTCT7' IndicatorId, 'No. of HIV negative pregnant women who were re-tested for HIV and received their results within this current pregnancy' IndicatorDescription, 55 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -3311,7 +3701,7 @@
         <v>select 56 IndicatorSerial , 'PMTCT8' IndicatorId, 'No. of HIV negative pregnant women who were re-tested for HIV and tested HIV positive within this current pregnancy' IndicatorDescription, 56 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -3336,7 +3726,7 @@
         <v>select 57 IndicatorSerial , 'PMTCT11' IndicatorId, 'Number of HIV positive pregnant women  on HAART (Lifelong ART, Including option B+)' IndicatorDescription, 57 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -3361,7 +3751,7 @@
         <v>select 58 IndicatorSerial , 'PMTCT11a' IndicatorId, 'Sub-Disag of Life-long ART: Newly initiated on treatment during the current pregnancy' IndicatorDescription, 58 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -3386,7 +3776,7 @@
         <v>select 59 IndicatorSerial , 'PMTCT11b' IndicatorId, 'Sub-Disag of Life-long ART: Already on treatment at the beginning of the current pregnancy' IndicatorDescription, 59 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -3411,7 +3801,7 @@
         <v>select 60 IndicatorSerial , 'PMTCT9' IndicatorId, 'Number of HIV positive pregnant women checked for CD4 as baseline' IndicatorDescription, 60 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -3436,7 +3826,7 @@
         <v>select 61 IndicatorSerial , 'PMTCT16' IndicatorId, 'Total number of infants born at this site this month' IndicatorDescription, 61 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -3461,7 +3851,7 @@
         <v>select 62 IndicatorSerial , 'PMTCT17' IndicatorId, 'Total number of infants born to HIV positive women at this site this month' IndicatorDescription, 62 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>102</v>
       </c>
@@ -3486,7 +3876,7 @@
         <v>select 63 IndicatorSerial , 'PMTCT18' IndicatorId, 'Number of HIV Exposed Infants (HEI)  who received ARV prophylaxis for PMTCT (Niverapine - NVP)' IndicatorDescription, 63 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -3511,7 +3901,7 @@
         <v>select 64 IndicatorSerial , 'PMTCT19' IndicatorId, 'Number of HEI who started cotrimoxazole prophylaxis (CTX) at 6 weeks' IndicatorDescription, 64 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -3536,7 +3926,7 @@
         <v>select 65 IndicatorSerial , 'PMTCT18_a' IndicatorId, 'NumberÂ ofÂ infantsÂ bornÂ toÂ HIV positiveÂ womenÂ whoÂ receivedÂ HIV virological testing at 6 weeks  ofÂ birth' IndicatorDescription, 65 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -3561,7 +3951,7 @@
         <v>select 66 IndicatorSerial , 'PMTCT19_a' IndicatorId, 'Number of infants born to HIV positive women who received HIV virological testing in the first 6 months of birth' IndicatorDescription, 66 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>102</v>
       </c>
@@ -3586,7 +3976,7 @@
         <v>select 67 IndicatorSerial , 'PMTCT20' IndicatorId, 'Number of infants born to HIV positive women who received HIV virological testing in the first 12 months of birth' IndicatorDescription, 67 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>102</v>
       </c>
@@ -3611,7 +4001,7 @@
         <v>select 68 IndicatorSerial , 'PMTCT22' IndicatorId, 'Number of infants born to HIV positive women who received HIV virological testing in the first 18 months of birth' IndicatorDescription, 68 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>102</v>
       </c>
@@ -3636,7 +4026,7 @@
         <v>select 69 IndicatorSerial , 'PMTCT23' IndicatorId, 'Number of infants with a   positive virological test  within 12 months' IndicatorDescription, 69 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>102</v>
       </c>
@@ -3661,7 +4051,7 @@
         <v>select 70 IndicatorSerial , 'PMTCT24' IndicatorId, 'Number of HIV-exposed infants registered in the birth cohort who are suppose to be discharge this (including transfer-ins) found in the mother baby tracking register.' IndicatorDescription, 70 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>102</v>
       </c>
@@ -3686,7 +4076,7 @@
         <v>select 71 IndicatorSerial , 'PMTCT24_a' IndicatorId, 'Sub-Disagg - In care but no test Done' IndicatorDescription, 71 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>102</v>
       </c>
@@ -3711,7 +4101,7 @@
         <v>select 72 IndicatorSerial , 'PMTCT24_b' IndicatorId, 'Sub-Disagg - Lost to follow-up' IndicatorDescription, 72 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>102</v>
       </c>
@@ -3736,7 +4126,7 @@
         <v>select 73 IndicatorSerial , 'PMTCT24_c' IndicatorId, 'Sub-Disagg - Died' IndicatorDescription, 73 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>102</v>
       </c>
@@ -3761,7 +4151,7 @@
         <v>select 74 IndicatorSerial , 'PMTCT24_d' IndicatorId, 'Sub-Disagg - Transferred out' IndicatorDescription, 74 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -3786,7 +4176,7 @@
         <v>select 75 IndicatorSerial , 'PMTCT25' IndicatorId, 'Number of HIV-exposed infants registered in the birth cohort who have been discharged with HIV negative Final Outcome results (including transfer-ins) found in the mother baby tracking register.' IndicatorDescription, 75 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>102</v>
       </c>
@@ -3811,7 +4201,7 @@
         <v>select 76 IndicatorSerial , 'PMTCT25_a' IndicatorId, 'Sub-Disaggregation of HIV negative infants - HIV Negative  not breastfeeding' IndicatorDescription, 76 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>102</v>
       </c>
@@ -3836,7 +4226,7 @@
         <v>select 77 IndicatorSerial , 'PMTCT25_b' IndicatorId, 'Sub-Disaggregation of HIV negative infants - HIV Negative who are still breastfeeding' IndicatorDescription, 77 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>102</v>
       </c>
@@ -3861,7 +4251,7 @@
         <v>select 78 IndicatorSerial , 'PMTCT25_c' IndicatorId, 'Sub-Disaggregation of HIV negative infants - HIV Negative breastfeeding status unknown' IndicatorDescription, 78 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -3886,7 +4276,7 @@
         <v>select 79 IndicatorSerial , 'PMTCT26' IndicatorId, 'Number of HIV-exposed infants with a documented outcome by 18 months of age disaggregated by outcome type.' IndicatorDescription, 79 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>102</v>
       </c>
@@ -3911,7 +4301,7 @@
         <v>select 80 IndicatorSerial , 'PMTCT26_a' IndicatorId, 'Sub-Disagg-HIV positive infants' IndicatorDescription, 80 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -3936,7 +4326,7 @@
         <v>select 81 IndicatorSerial , 'PMTCT26_b' IndicatorId, 'Sub-Disagg-HIV positive infants linked to ART' IndicatorDescription, 81 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -3961,7 +4351,7 @@
         <v>select 82 IndicatorSerial , 'PMTCT26_c' IndicatorId, 'Sub-Disagg-HIV negative infants' IndicatorDescription, 82 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>102</v>
       </c>
@@ -3986,7 +4376,7 @@
         <v>select 83 IndicatorSerial , 'PMTCT29' IndicatorId, 'No. of HIV-exposed infants who were on exclusively breastfeeding (EBF) at or around 3 months' IndicatorDescription, 83 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -4011,7 +4401,7 @@
         <v>select 84 IndicatorSerial , 'PMTCT30' IndicatorId, 'No. of HIV-exposed infants who were on replacement feeding (ERF)  at or around 3 months - (no breast milk at all)' IndicatorDescription, 84 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -4036,7 +4426,7 @@
         <v>select 85 IndicatorSerial , 'PMTCT31' IndicatorId, 'No. of HIV-exposed infants who were on mixed feeding  at or around 3 months' IndicatorDescription, 85 zPosition , 3 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -4061,7 +4451,7 @@
         <v>select 86 IndicatorSerial , 'FP1' IndicatorId, 'Number of new acceptors of modern contraception by method type (disaggregated by gender and age)' IndicatorDescription, 86 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -4086,7 +4476,7 @@
         <v>select 87 IndicatorSerial , 'FP1_a' IndicatorId, 'Disagg. by Method Type-Male Condoms' IndicatorDescription, 87 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>175</v>
       </c>
@@ -4111,7 +4501,7 @@
         <v>select 88 IndicatorSerial , 'FP1_b' IndicatorId, 'Disagg. by Method Type-Female Condoms' IndicatorDescription, 88 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -4136,7 +4526,7 @@
         <v>select 89 IndicatorSerial , 'FP1_c' IndicatorId, 'Disagg. by Method Type-Combined oral contraceptives' IndicatorDescription, 89 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>175</v>
       </c>
@@ -4161,7 +4551,7 @@
         <v>select 90 IndicatorSerial , 'FP1_d' IndicatorId, 'Disagg. by Method Type-Progesterone only pill' IndicatorDescription, 90 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -4186,7 +4576,7 @@
         <v>select 91 IndicatorSerial , 'FP1_e' IndicatorId, 'Disagg. by Method Type-Depo-Provera' IndicatorDescription, 91 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -4211,7 +4601,7 @@
         <v>select 92 IndicatorSerial , 'FP1_f' IndicatorId, 'Disagg. by Method Type-Intrauterine Devices (IUD)- Interval' IndicatorDescription, 92 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>175</v>
       </c>
@@ -4236,7 +4626,7 @@
         <v>select 93 IndicatorSerial , 'FP1_g' IndicatorId, 'Disagg. by Method Type-Postpatum Intrauterine Devices (IUD) within 48 hours of delivery' IndicatorDescription, 93 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -4261,7 +4651,7 @@
         <v>select 94 IndicatorSerial , 'FP1_h' IndicatorId, 'Disagg. by Method Type-Subderminal implants (jaddel)' IndicatorDescription, 94 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>175</v>
       </c>
@@ -4286,7 +4676,7 @@
         <v>select 95 IndicatorSerial , 'FP1_i' IndicatorId, 'Disagg. by Method Type-Noristerat/Noresterat injection' IndicatorDescription, 95 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>175</v>
       </c>
@@ -4311,7 +4701,7 @@
         <v>select 96 IndicatorSerial , 'FP1_j' IndicatorId, 'Disagg. by Method Type-Female sterilization' IndicatorDescription, 96 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>175</v>
       </c>
@@ -4336,7 +4726,7 @@
         <v>select 97 IndicatorSerial , 'FP1_k' IndicatorId, 'Disagg. by Method Type-Male sterilization' IndicatorDescription, 97 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>175</v>
       </c>
@@ -4361,7 +4751,7 @@
         <v>select 98 IndicatorSerial , 'FP1_m' IndicatorId, 'Disagg. by Method Type-TOTAL' IndicatorDescription, 98 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>175</v>
       </c>
@@ -4386,7 +4776,7 @@
         <v>select 99 IndicatorSerial , 'FP2' IndicatorId, 'Number of clients receiving or maintaining a modern FP method (disaggregated by age, gender and type of method)' IndicatorDescription, 99 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>175</v>
       </c>
@@ -4411,7 +4801,7 @@
         <v>select 100 IndicatorSerial , 'FP2_a' IndicatorId, 'Disagg. by method type-Male Condoms' IndicatorDescription, 100 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>175</v>
       </c>
@@ -4436,7 +4826,7 @@
         <v>select 101 IndicatorSerial , 'FP2_b' IndicatorId, 'Disagg. by method type-Female Condoms' IndicatorDescription, 101 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>175</v>
       </c>
@@ -4461,7 +4851,7 @@
         <v>select 102 IndicatorSerial , 'FP2_c' IndicatorId, 'Disagg. by method type-Combined oral contraceptives' IndicatorDescription, 102 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>175</v>
       </c>
@@ -4486,7 +4876,7 @@
         <v>select 103 IndicatorSerial , 'FP2_d' IndicatorId, 'Disagg. by method type-Progesterone only pill' IndicatorDescription, 103 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>175</v>
       </c>
@@ -4511,7 +4901,7 @@
         <v>select 104 IndicatorSerial , 'FP2_e' IndicatorId, 'Disagg. by method type-Depo-Provera' IndicatorDescription, 104 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>175</v>
       </c>
@@ -4536,7 +4926,7 @@
         <v>select 105 IndicatorSerial , 'FP2_f' IndicatorId, 'Disagg. by method type-Intrauterine Devices (IUD)- Interval' IndicatorDescription, 105 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>175</v>
       </c>
@@ -4561,7 +4951,7 @@
         <v>select 106 IndicatorSerial , 'FP2_g' IndicatorId, 'Disagg. by method type-Postpatum Intrauterine Devices (IUD) within 48 hours of delivery' IndicatorDescription, 106 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>175</v>
       </c>
@@ -4586,7 +4976,7 @@
         <v>select 107 IndicatorSerial , 'FP2_h' IndicatorId, 'Disagg. by method type-Subderminal implants (jaddel)' IndicatorDescription, 107 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>175</v>
       </c>
@@ -4611,7 +5001,7 @@
         <v>select 108 IndicatorSerial , 'FP2_i' IndicatorId, 'Disagg. by method type-Noristerat/Noresterat injection' IndicatorDescription, 108 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>175</v>
       </c>
@@ -4636,7 +5026,7 @@
         <v>select 109 IndicatorSerial , 'FP2_j' IndicatorId, 'Disagg. by method type-Female sterilization' IndicatorDescription, 109 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>175</v>
       </c>
@@ -4661,7 +5051,7 @@
         <v>select 110 IndicatorSerial , 'FP2_k' IndicatorId, 'Disagg. by method type-Male sterilization' IndicatorDescription, 110 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>175</v>
       </c>
@@ -4686,7 +5076,7 @@
         <v>select 111 IndicatorSerial , 'FP2_m' IndicatorId, 'Disagg. by method type-TOTAL' IndicatorDescription, 111 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>175</v>
       </c>
@@ -4711,7 +5101,7 @@
         <v>select 112 IndicatorSerial , 'FP3a' IndicatorId, 'Number of FP new acceptors of modern contraception who received HTC and received their HIV results from FP service delivery point (disaggregated by gender and age)' IndicatorDescription, 112 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>175</v>
       </c>
@@ -4736,7 +5126,7 @@
         <v>select 113 IndicatorSerial , 'FP3b' IndicatorId, 'Number of  FP new acceptors of modern contraception who tested HIV+ from FP service delivery point (disaggregated by gender and age)' IndicatorDescription, 113 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>175</v>
       </c>
@@ -4761,7 +5151,7 @@
         <v>select 114 IndicatorSerial , 'FP4' IndicatorId, 'Number of FP clients switching from short term to long term methods (disaggregated by method type: Jaddel or IUD)' IndicatorDescription, 114 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>175</v>
       </c>
@@ -4786,7 +5176,7 @@
         <v>select 115 IndicatorSerial , 'FP5' IndicatorId, 'Number of postpartum women accessing Family Planning disaggregated by timing from birth to one year' IndicatorDescription, 115 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>175</v>
       </c>
@@ -4811,7 +5201,7 @@
         <v>select 116 IndicatorSerial , 'FP5_a' IndicatorId, 'Disagg. By time from birth-48 hours' IndicatorDescription, 116 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>175</v>
       </c>
@@ -4836,7 +5226,7 @@
         <v>select 117 IndicatorSerial , 'FP5_b' IndicatorId, 'Disagg. By time from birth-6 weeks' IndicatorDescription, 117 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>175</v>
       </c>
@@ -4861,7 +5251,7 @@
         <v>select 118 IndicatorSerial , 'FP5_c' IndicatorId, 'Disagg. By time from birth-6 months' IndicatorDescription, 118 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>175</v>
       </c>
@@ -4886,7 +5276,7 @@
         <v>select 119 IndicatorSerial , 'FP5_d' IndicatorId, 'Disagg. By time from birth-12 months' IndicatorDescription, 119 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>175</v>
       </c>
@@ -4911,7 +5301,7 @@
         <v>select 120 IndicatorSerial , 'FP5_e' IndicatorId, 'Disagg. By time from birth-TOTAL' IndicatorDescription, 120 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>175</v>
       </c>
@@ -4936,7 +5326,7 @@
         <v>select 121 IndicatorSerial , 'FP6' IndicatorId, 'Number of clients started on dual protection (disaggregated by HIV status)' IndicatorDescription, 121 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>175</v>
       </c>
@@ -4961,7 +5351,7 @@
         <v>select 122 IndicatorSerial , 'FP7' IndicatorId, 'Number of women seeking FP who were already pregnant (disaggregated by HIV status)' IndicatorDescription, 122 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>175</v>
       </c>
@@ -4986,7 +5376,7 @@
         <v>select 123 IndicatorSerial , 'FP8' IndicatorId, 'Number FP clients receiving FP services as a couple' IndicatorDescription, 123 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>175</v>
       </c>
@@ -5011,7 +5401,7 @@
         <v>select 124 IndicatorSerial , 'FP9' IndicatorId, 'Number of clients referred from community to facility for FP' IndicatorDescription, 124 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>175</v>
       </c>
@@ -5036,7 +5426,7 @@
         <v>select 125 IndicatorSerial , 'FP10' IndicatorId, 'Number of clients referred from FP to CECAP' IndicatorDescription, 125 zPosition , 6 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>256</v>
       </c>
@@ -5061,7 +5451,7 @@
         <v>select 126 IndicatorSerial , 'PwP1' IndicatorId, 'Number of People Living with HIV/AIDS (PLHIV) NEWLY reached with a minimum package of PWP interventions in a facility and community-based setting' IndicatorDescription, 126 zPosition , 7 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>256</v>
       </c>
@@ -5086,7 +5476,7 @@
         <v>select 127 IndicatorSerial , 'PwP2' IndicatorId, 'Total number of People Living with HIV/AIDS (PLHIV) EVER reached with a minimum package of PWP interventions in a facility and community-based setting' IndicatorDescription, 127 zPosition , 7 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -5111,7 +5501,7 @@
         <v>select 128 IndicatorSerial , 'PwP2a' IndicatorId, 'Number of PLHIV reached with PWP interventions in a facility setting this month' IndicatorDescription, 128 zPosition , 7 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -5136,7 +5526,7 @@
         <v>select 129 IndicatorSerial , 'PwP2b' IndicatorId, 'Number of PLHIV reached with PWP interventions in a community/home-based  care setting this month' IndicatorDescription, 129 zPosition , 7 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>265</v>
       </c>
@@ -5157,11 +5547,11 @@
         <v>130</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" ref="G131:G168" si="7">"select "&amp;D131&amp;" IndicatorSerial , '"&amp;B131&amp;"' IndicatorId, '"&amp;C131&amp;"' IndicatorDescription, "&amp;F131&amp;" zPosition , "&amp;E131&amp;" ProgramAreaID union"</f>
+        <f t="shared" ref="G131:G194" si="7">"select "&amp;D131&amp;" IndicatorSerial , '"&amp;B131&amp;"' IndicatorId, '"&amp;C131&amp;"' IndicatorDescription, "&amp;F131&amp;" zPosition , "&amp;E131&amp;" ProgramAreaID union"</f>
         <v>select 130 IndicatorSerial , 'CS1a' IndicatorId, 'Number of HIV postive Individuals who received Pre-ART Care services (including Pregnant women) which are clinical assessment (WHO staging) OR CD4 count OR viral load - Newly enrolled to care services' IndicatorDescription, 130 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>265</v>
       </c>
@@ -5186,7 +5576,7 @@
         <v>select 131 IndicatorSerial , 'CS1b' IndicatorId, 'No of HIV positive pregnant women newly enrolled into HIV care and support services- Fraction of CS1a' IndicatorDescription, 131 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>265</v>
       </c>
@@ -5211,7 +5601,7 @@
         <v>select 132 IndicatorSerial , 'CS2a' IndicatorId, 'Number of HIV positive adults and children who received at least one of the following this month: clinical assessment (WHO staging) OR CD4 count OR viral load' IndicatorDescription, 132 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>265</v>
       </c>
@@ -5236,7 +5626,7 @@
         <v>select 133 IndicatorSerial , 'CS2b' IndicatorId, 'Number of existing HIV-positive adults and children receiving a minimum of one clinical care service this month, (these are the total number of clients existing and active in a facility and receiving clinical care only)' IndicatorDescription, 133 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>265</v>
       </c>
@@ -5261,7 +5651,7 @@
         <v>select 134 IndicatorSerial , 'CS3' IndicatorId, 'Number of HIV positive adults and children who had CD4 count done this month' IndicatorDescription, 134 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>265</v>
       </c>
@@ -5286,7 +5676,7 @@
         <v>select 135 IndicatorSerial , 'CS5' IndicatorId, 'No. of HIV positive patients screened for chronic conditions this month: (Diabetes Mellitus, Hypertension, TB)' IndicatorDescription, 135 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>265</v>
       </c>
@@ -5311,7 +5701,7 @@
         <v>select 136 IndicatorSerial , 'CS6' IndicatorId, 'Number of community/home-based care givers trained in clinical, preventive and support care' IndicatorDescription, 136 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>265</v>
       </c>
@@ -5336,7 +5726,7 @@
         <v>select 137 IndicatorSerial , 'CS7' IndicatorId, 'Number of active care givers in the palliative/home based care and OVC care program this month' IndicatorDescription, 137 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>265</v>
       </c>
@@ -5361,7 +5751,7 @@
         <v>select 138 IndicatorSerial , 'CS8' IndicatorId, 'Number of HIV-positive persons receiving cotrimoxazole prophylaxis this month' IndicatorDescription, 138 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>265</v>
       </c>
@@ -5386,7 +5776,7 @@
         <v>select 139 IndicatorSerial , 'CS9a' IndicatorId, 'Number of HIV-positive patients  who were nutritionally assessed and found to be clinically malnourished during the reporting period.' IndicatorDescription, 139 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>265</v>
       </c>
@@ -5411,7 +5801,7 @@
         <v>select 140 IndicatorSerial , 'CS9b' IndicatorId, 'Number of HIV-positive clinically malnourisheds adult  and children who received therapeutic or supplementary food this month' IndicatorDescription, 140 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>265</v>
       </c>
@@ -5436,7 +5826,7 @@
         <v>select 141 IndicatorSerial , 'CS9c' IndicatorId, 'Number of PLHIV who were nutritionally assessed via anthropometric measurement' IndicatorDescription, 141 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>265</v>
       </c>
@@ -5461,7 +5851,7 @@
         <v>select 142 IndicatorSerial , 'CS9d' IndicatorId, 'Number of PLHIV provided with home based care services.' IndicatorDescription, 142 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>265</v>
       </c>
@@ -5486,7 +5876,7 @@
         <v>select 143 IndicatorSerial , 'CS10' IndicatorId, 'Number of HIV-positive patients who were screened for TB this month' IndicatorDescription, 143 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>265</v>
       </c>
@@ -5511,7 +5901,7 @@
         <v>select 144 IndicatorSerial , 'CS10a' IndicatorId, 'Number of HIV-positive patients who were screened for TB at the health facility this month' IndicatorDescription, 144 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>265</v>
       </c>
@@ -5536,7 +5926,7 @@
         <v>select 145 IndicatorSerial , 'CS10b' IndicatorId, 'Number of HIV-positive patients who were screened for TB in a  community setting this month' IndicatorDescription, 145 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>265</v>
       </c>
@@ -5561,7 +5951,7 @@
         <v>select 146 IndicatorSerial , 'CS11' IndicatorId, 'Number of HIV-positive patients who were screened for TB in HIV care or treatment setting' IndicatorDescription, 146 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>265</v>
       </c>
@@ -5586,7 +5976,7 @@
         <v>select 147 IndicatorSerial , 'CS11a' IndicatorId, 'Number of HIV-positive patients who were diagonised with active TB disease' IndicatorDescription, 147 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>265</v>
       </c>
@@ -5611,7 +6001,7 @@
         <v>select 148 IndicatorSerial , 'CS11b' IndicatorId, 'Number of PLHIV newly enrolled in HIV clinical care who start isoniazid preventative therapy (IPT)' IndicatorDescription, 148 zPosition , 8 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>304</v>
       </c>
@@ -5636,7 +6026,7 @@
         <v>select 149 IndicatorSerial , 'MC1' IndicatorId, 'Total number of males circumcised as part of the minimum package of MC for HIV prevention services (MC1 = MC1a + MC1b)' IndicatorDescription, 149 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>304</v>
       </c>
@@ -5661,7 +6051,7 @@
         <v>select 150 IndicatorSerial , 'MC1a' IndicatorId, 'Number of males circumcised as part of the minimum package of MC for HIV prevention services (Static MC site)' IndicatorDescription, 150 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>304</v>
       </c>
@@ -5686,7 +6076,7 @@
         <v>select 151 IndicatorSerial , 'MC1b' IndicatorId, 'Number of males circumcised as part of the minimum package of MC for HIV prevention services (Mobile Site)' IndicatorDescription, 151 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>304</v>
       </c>
@@ -5711,7 +6101,7 @@
         <v>select 152 IndicatorSerial , 'MC1c' IndicatorId, 'Number circumcised by surgical technique (forceps guided, dorsal slit, sleeve resection)' IndicatorDescription, 152 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>304</v>
       </c>
@@ -5736,7 +6126,7 @@
         <v>select 153 IndicatorSerial , 'MC2' IndicatorId, 'Number of circumcised clients experiencing at least one moderate or severe adverse event (AE) during or following surgery, within the reporting period (MC2 = MC2a + MC2b)' IndicatorDescription, 153 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>304</v>
       </c>
@@ -5761,7 +6151,7 @@
         <v>select 154 IndicatorSerial , 'MC2a' IndicatorId, 'Number of VMMC clients with one or more moderate or severe surgical intra-operative AE(s)' IndicatorDescription, 154 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>304</v>
       </c>
@@ -5786,7 +6176,7 @@
         <v>select 155 IndicatorSerial , 'MC2b' IndicatorId, 'Number of VMMC clients with one or more moderate or severe surgical post-operative AE(s)' IndicatorDescription, 155 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>304</v>
       </c>
@@ -5811,7 +6201,7 @@
         <v>select 156 IndicatorSerial , 'MC2c' IndicatorId, 'Number of clients with one or more moderate surgical post-operative AE(s), but no severe surgical post-operative AE(s)' IndicatorDescription, 156 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>304</v>
       </c>
@@ -5836,7 +6226,7 @@
         <v>select 157 IndicatorSerial , 'MC2d' IndicatorId, 'Number of clients with one or more severe surgical intra-operative AE(s)' IndicatorDescription, 157 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>304</v>
       </c>
@@ -5861,7 +6251,7 @@
         <v>select 158 IndicatorSerial , 'MC2e' IndicatorId, 'Number of surgically circumcised clients who returned at least once for follow-up care within 14 days of their circumcision surgery' IndicatorDescription, 158 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>304</v>
       </c>
@@ -5886,7 +6276,7 @@
         <v>select 159 IndicatorSerial , 'MC2f' IndicatorId, 'Number of surgically circumcised clients who did NOT return for follow-up care within 14 days of their circumcision surgery' IndicatorDescription, 159 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>304</v>
       </c>
@@ -5911,7 +6301,7 @@
         <v>select 160 IndicatorSerial , 'MC3' IndicatorId, 'Number of MC clients pre-test counseled, tested and collected HIV test results at MC centers' IndicatorDescription, 160 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>304</v>
       </c>
@@ -5925,7 +6315,7 @@
         <v>161</v>
       </c>
       <c r="E162">
-        <f t="shared" ref="E162:E168" si="8">VLOOKUP(A162,progarea,2,FALSE)</f>
+        <f t="shared" ref="E162:E199" si="8">VLOOKUP(A162,progarea,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F162">
@@ -5936,7 +6326,7 @@
         <v>select 161 IndicatorSerial , 'MC3a' IndicatorId, 'Number of HIV negative clients (tested HIV negative at VMMC site)' IndicatorDescription, 161 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>304</v>
       </c>
@@ -5961,7 +6351,7 @@
         <v>select 162 IndicatorSerial , 'MC3b' IndicatorId, 'Number of clients with undocumented/indeterminate HIV status or not tested for HIV at VMMC site.' IndicatorDescription, 162 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>304</v>
       </c>
@@ -5986,7 +6376,7 @@
         <v>select 163 IndicatorSerial , 'MC4' IndicatorId, 'Number of MC clients testing positive for HIV and collecting results at MC centers' IndicatorDescription, 163 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>304</v>
       </c>
@@ -6011,7 +6401,7 @@
         <v>select 164 IndicatorSerial , 'MC4a' IndicatorId, 'Number of MC clients testing positive for HIV, collecting results and referred for clinical care beyond MC' IndicatorDescription, 164 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>304</v>
       </c>
@@ -6036,7 +6426,7 @@
         <v>select 165 IndicatorSerial , 'MC4b' IndicatorId, 'Number of VMMC clients who reached the the referral service (ART, STI)' IndicatorDescription, 165 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>304</v>
       </c>
@@ -6061,7 +6451,7 @@
         <v>select 166 IndicatorSerial , 'MC7' IndicatorId, 'Number of HIV-positive men circumcised (tested at MC site) who were referred for HIV care' IndicatorDescription, 166 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>304</v>
       </c>
@@ -6086,6 +6476,782 @@
         <v>select 167 IndicatorSerial , 'MC12' IndicatorId, 'Number of males circumcised within the reporting period who return at least once for post-operative follow-up care (routine or emergent) within 48hours of surgery' IndicatorDescription, 167 zPosition , 2 ProgramAreaID union</v>
       </c>
     </row>
+    <row r="169" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D169" s="1">
+        <v>168</v>
+      </c>
+      <c r="E169" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F169">
+        <v>168</v>
+      </c>
+      <c r="G169" t="str">
+        <f t="shared" si="7"/>
+        <v>select 168 IndicatorSerial , 'CECAP 1' IndicatorId, 'Number of clients who received a VIA screening (Total)' IndicatorDescription, 168 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D170" s="1">
+        <v>169</v>
+      </c>
+      <c r="E170" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F170">
+        <v>169</v>
+      </c>
+      <c r="G170" t="str">
+        <f t="shared" si="7"/>
+        <v>select 169 IndicatorSerial , 'CECAP 2' IndicatorId, 'Number of  new women screened using VIA (New)' IndicatorDescription, 169 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D171" s="1">
+        <v>170</v>
+      </c>
+      <c r="E171" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F171">
+        <v>170</v>
+      </c>
+      <c r="G171" t="str">
+        <f t="shared" si="7"/>
+        <v>select 170 IndicatorSerial , 'CECAP 3' IndicatorId, 'Number of clients who had HIV test done and received results (during screening) this month' IndicatorDescription, 170 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D172" s="1">
+        <v>171</v>
+      </c>
+      <c r="E172" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F172">
+        <v>171</v>
+      </c>
+      <c r="G172" t="str">
+        <f t="shared" si="7"/>
+        <v>select 171 IndicatorSerial , 'CECAP 4' IndicatorId, 'Number of New women screened using VIA and tested for HIV' IndicatorDescription, 171 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D173" s="1">
+        <v>172</v>
+      </c>
+      <c r="E173" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F173">
+        <v>172</v>
+      </c>
+      <c r="G173" t="str">
+        <f t="shared" si="7"/>
+        <v>select 172 IndicatorSerial , 'CECAP 5' IndicatorId, 'Total Number of women screen for VIA with Positive HIV test result.' IndicatorDescription, 172 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D174" s="1">
+        <v>173</v>
+      </c>
+      <c r="E174" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F174">
+        <v>173</v>
+      </c>
+      <c r="G174" t="str">
+        <f t="shared" si="7"/>
+        <v>select 173 IndicatorSerial , 'CECAP 6' IndicatorId, 'Number of clients with NEGATIVE VIA result' IndicatorDescription, 173 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D175" s="1">
+        <v>174</v>
+      </c>
+      <c r="E175" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F175">
+        <v>174</v>
+      </c>
+      <c r="G175" t="str">
+        <f t="shared" si="7"/>
+        <v>select 174 IndicatorSerial , 'CECAP 7' IndicatorId, 'Number of clients with POSITIVE VIA result' IndicatorDescription, 174 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D176" s="1">
+        <v>175</v>
+      </c>
+      <c r="E176" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F176">
+        <v>175</v>
+      </c>
+      <c r="G176" t="str">
+        <f t="shared" si="7"/>
+        <v>select 175 IndicatorSerial , 'CECAP 8' IndicatorId, 'Number of clients with VIA today AND cryotherapy performed today. (SVA) ' IndicatorDescription, 175 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D177" s="1">
+        <v>176</v>
+      </c>
+      <c r="E177" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F177">
+        <v>176</v>
+      </c>
+      <c r="G177" t="str">
+        <f t="shared" si="7"/>
+        <v>select 176 IndicatorSerial , 'CECAP 9' IndicatorId, 'Number of clients with previously postponed cryotherapy performed today' IndicatorDescription, 176 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D178" s="1">
+        <v>177</v>
+      </c>
+      <c r="E178" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F178">
+        <v>177</v>
+      </c>
+      <c r="G178" t="str">
+        <f t="shared" si="7"/>
+        <v>select 177 IndicatorSerial , 'CECAP 10' IndicatorId, 'Number of clients with VIA today AND cryotherapy postponed' IndicatorDescription, 177 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D179" s="1">
+        <v>178</v>
+      </c>
+      <c r="E179" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F179">
+        <v>178</v>
+      </c>
+      <c r="G179" t="str">
+        <f t="shared" si="7"/>
+        <v>select 178 IndicatorSerial , 'CECAP 11' IndicatorId, 'Number of clients referred for large lesions' IndicatorDescription, 178 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D180" s="1">
+        <v>179</v>
+      </c>
+      <c r="E180" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F180">
+        <v>179</v>
+      </c>
+      <c r="G180" t="str">
+        <f t="shared" si="7"/>
+        <v>select 179 IndicatorSerial , 'CECAP 12' IndicatorId, 'Number of clients with suspected cancer' IndicatorDescription, 179 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D181" s="1">
+        <v>180</v>
+      </c>
+      <c r="E181" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F181">
+        <v>180</v>
+      </c>
+      <c r="G181" t="str">
+        <f t="shared" si="7"/>
+        <v>select 180 IndicatorSerial , 'CECAP 13' IndicatorId, 'Number of clients with a post-treatment complication ' IndicatorDescription, 180 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D182" s="1">
+        <v>181</v>
+      </c>
+      <c r="E182" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F182">
+        <v>181</v>
+      </c>
+      <c r="G182" t="str">
+        <f t="shared" si="7"/>
+        <v>select 181 IndicatorSerial , 'CECAP 14' IndicatorId, 'Number new women treated with cryotherapy' IndicatorDescription, 181 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D183" s="1">
+        <v>182</v>
+      </c>
+      <c r="E183" s="1">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F183">
+        <v>182</v>
+      </c>
+      <c r="G183" t="str">
+        <f t="shared" si="7"/>
+        <v>select 182 IndicatorSerial , 'CECAP 15' IndicatorId, 'Total number of unique clients seen this month' IndicatorDescription, 182 zPosition , 10 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" s="1" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D184" s="1">
+        <v>183</v>
+      </c>
+      <c r="E184" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F184">
+        <v>183</v>
+      </c>
+      <c r="G184" t="str">
+        <f t="shared" si="7"/>
+        <v>select 183 IndicatorSerial , 'CT1' IndicatorId, 'Total No. of clients who were counselled and tested for HIV and received their test results  at the facility Including PITC this month.' IndicatorDescription, 183 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D185" s="1">
+        <v>184</v>
+      </c>
+      <c r="E185" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F185">
+        <v>184</v>
+      </c>
+      <c r="G185" t="str">
+        <f t="shared" si="7"/>
+        <v>select 184 IndicatorSerial , 'CT1a.1' IndicatorId, 'No. of clients who received counseling and testing (CT) services for HIV and received their test results this month' IndicatorDescription, 184 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D186" s="1">
+        <v>185</v>
+      </c>
+      <c r="E186" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F186">
+        <v>185</v>
+      </c>
+      <c r="G186" t="str">
+        <f t="shared" si="7"/>
+        <v>select 185 IndicatorSerial , 'CT1b' IndicatorId, 'Number of all clients who tested  HIV positive for HIV and collected test results.' IndicatorDescription, 185 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D187" s="1">
+        <v>186</v>
+      </c>
+      <c r="E187" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F187">
+        <v>186</v>
+      </c>
+      <c r="G187" t="str">
+        <f t="shared" si="7"/>
+        <v>select 186 IndicatorSerial , 'CT1b.1' IndicatorId, 'Number of clients who tested as couple and collected test results at this facility this month.' IndicatorDescription, 186 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D188" s="1">
+        <v>187</v>
+      </c>
+      <c r="E188" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F188">
+        <v>187</v>
+      </c>
+      <c r="G188" t="str">
+        <f t="shared" si="7"/>
+        <v>select 187 IndicatorSerial , 'CT1c' IndicatorId, 'Numbner of HIV DISCONDANT couples who received test results. (Count Females only).' IndicatorDescription, 187 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D189" s="1">
+        <v>188</v>
+      </c>
+      <c r="E189" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F189">
+        <v>188</v>
+      </c>
+      <c r="G189" t="str">
+        <f t="shared" si="7"/>
+        <v>select 188 IndicatorSerial , 'CT1c.1' IndicatorId, 'Number of clients who were re-tested for HIV and received there results' IndicatorDescription, 188 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="D190" s="1">
+        <v>189</v>
+      </c>
+      <c r="E190" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F190">
+        <v>189</v>
+      </c>
+      <c r="G190" t="str">
+        <f t="shared" si="7"/>
+        <v>select 189 IndicatorSerial , 'CT1d' IndicatorId, 'Number of clients who re-tested and tested positive for HIV.' IndicatorDescription, 189 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="D191" s="1">
+        <v>190</v>
+      </c>
+      <c r="E191" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F191">
+        <v>190</v>
+      </c>
+      <c r="G191" t="str">
+        <f t="shared" si="7"/>
+        <v>select 190 IndicatorSerial , 'CT.e' IndicatorId, 'Numbner of clients who Tested for HIV through PITC (Total of PMTCT,STI,TB,MC,CECAP,FP)' IndicatorDescription, 190 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D192" s="1">
+        <v>191</v>
+      </c>
+      <c r="E192" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F192">
+        <v>191</v>
+      </c>
+      <c r="G192" t="str">
+        <f t="shared" si="7"/>
+        <v>select 191 IndicatorSerial , 'CT.e.1' IndicatorId, 'Number of clients who tested for HIV through PMTCT' IndicatorDescription, 191 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D193" s="1">
+        <v>192</v>
+      </c>
+      <c r="E193" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F193">
+        <v>192</v>
+      </c>
+      <c r="G193" t="str">
+        <f t="shared" si="7"/>
+        <v>select 192 IndicatorSerial , 'CT.e.2' IndicatorId, 'Number of clients who tested for HIV through TB' IndicatorDescription, 192 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D194" s="1">
+        <v>193</v>
+      </c>
+      <c r="E194" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F194">
+        <v>193</v>
+      </c>
+      <c r="G194" t="str">
+        <f t="shared" si="7"/>
+        <v>select 193 IndicatorSerial , 'CT.e.3' IndicatorId, 'Number of clients who tested for HIV through STI' IndicatorDescription, 193 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C195" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D195" s="1">
+        <v>194</v>
+      </c>
+      <c r="E195" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F195">
+        <v>194</v>
+      </c>
+      <c r="G195" t="str">
+        <f t="shared" ref="G195:G199" si="9">"select "&amp;D195&amp;" IndicatorSerial , '"&amp;B195&amp;"' IndicatorId, '"&amp;C195&amp;"' IndicatorDescription, "&amp;F195&amp;" zPosition , "&amp;E195&amp;" ProgramAreaID union"</f>
+        <v>select 194 IndicatorSerial , 'CT.e.4' IndicatorId, 'Number of clients who tested for HIV through FP' IndicatorDescription, 194 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A196" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D196" s="1">
+        <v>195</v>
+      </c>
+      <c r="E196" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F196">
+        <v>195</v>
+      </c>
+      <c r="G196" t="str">
+        <f t="shared" si="9"/>
+        <v>select 195 IndicatorSerial , 'CT.e.5' IndicatorId, 'Number of clients who tested for HIV through CECAP' IndicatorDescription, 195 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D197" s="1">
+        <v>196</v>
+      </c>
+      <c r="E197" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F197">
+        <v>196</v>
+      </c>
+      <c r="G197" t="str">
+        <f t="shared" si="9"/>
+        <v>select 196 IndicatorSerial , 'CT.e.6' IndicatorId, 'Number of clients who tested for HIV through VMMC' IndicatorDescription, 196 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D198" s="1">
+        <v>197</v>
+      </c>
+      <c r="E198" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F198">
+        <v>197</v>
+      </c>
+      <c r="G198" t="str">
+        <f t="shared" si="9"/>
+        <v>select 197 IndicatorSerial , 'CT.e.7' IndicatorId, 'Number of Clients who tested positive from PITC' IndicatorDescription, 197 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A199" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D199" s="1">
+        <v>198</v>
+      </c>
+      <c r="E199" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="F199">
+        <v>198</v>
+      </c>
+      <c r="G199" t="str">
+        <f t="shared" si="9"/>
+        <v>select 198 IndicatorSerial , 'CT.f' IndicatorId, 'Total number of clients referred for Pre ART Care Services this Months' IndicatorDescription, 198 zPosition , 9 ProgramAreaID union</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6093,20 +7259,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H9"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B10" sqref="B10:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -6126,7 +7292,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
@@ -6137,16 +7303,16 @@
         <v>304</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>350</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
@@ -6157,16 +7323,16 @@
         <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -6177,16 +7343,16 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>175</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>5</v>
       </c>
@@ -6197,16 +7363,16 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>256</v>
+        <v>349</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -6217,16 +7383,16 @@
         <v>175</v>
       </c>
       <c r="F7" t="s">
-        <v>304</v>
+        <v>102</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>7</v>
       </c>
@@ -6237,16 +7403,16 @@
         <v>256</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>256</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>8</v>
       </c>
@@ -6257,19 +7423,450 @@
         <v>265</v>
       </c>
       <c r="F9" t="s">
+        <v>304</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" t="s">
+        <v>350</v>
+      </c>
+      <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G9">
+      <c r="G11">
         <v>5</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H11" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F2:H9">
-    <sortCondition ref="F2:F9"/>
+  <sortState ref="F2:H11">
+    <sortCondition ref="F2:F11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="62.44140625" customWidth="1"/>
+    <col min="4" max="4" width="100.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"{"&amp;"""IndicatorId"":"""&amp;B2&amp;""","&amp;"""Indicator"":"""&amp;C2&amp;"""},"</f>
+        <v>{"IndicatorId":"CECAP 1","Indicator":"Number of clients who received a VIA screening (Total)"},</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D33" si="0">"{"&amp;"""IndicatorId"":"""&amp;B3&amp;""","&amp;"""Indicator"":"""&amp;C3&amp;"""},"</f>
+        <v>{"IndicatorId":"CECAP 2","Indicator":"Number of  new women screened using VIA (New)"},</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 3","Indicator":"Number of clients who had HIV test done and received results (during screening) this month"},</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>357</v>
+      </c>
+      <c r="C5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 4","Indicator":"Number of New women screened using VIA and tested for HIV"},</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>359</v>
+      </c>
+      <c r="C6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 5","Indicator":"Total Number of women screen for VIA with Positive HIV test result."},</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 6","Indicator":"Number of clients with NEGATIVE VIA result"},</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 7","Indicator":"Number of clients with POSITIVE VIA result"},</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>365</v>
+      </c>
+      <c r="C9" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 8","Indicator":"Number of clients with VIA today AND cryotherapy performed today. (SVA) "},</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>367</v>
+      </c>
+      <c r="C10" t="s">
+        <v>368</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 9","Indicator":"Number of clients with previously postponed cryotherapy performed today"},</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C11" t="s">
+        <v>370</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 10","Indicator":"Number of clients with VIA today AND cryotherapy postponed"},</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>371</v>
+      </c>
+      <c r="C12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 11","Indicator":"Number of clients referred for large lesions"},</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>373</v>
+      </c>
+      <c r="C13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 12","Indicator":"Number of clients with suspected cancer"},</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 13","Indicator":"Number of clients with a post-treatment complication "},</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>377</v>
+      </c>
+      <c r="C15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 14","Indicator":"Number new women treated with cryotherapy"},</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" t="s">
+        <v>380</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CECAP 15","Indicator":"Total number of unique clients seen this month"},</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>381</v>
+      </c>
+      <c r="C18" t="s">
+        <v>382</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1","Indicator":"Total No. of clients who were counselled and tested for HIV and received their test results  at the facility Including PITC this month."},</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>383</v>
+      </c>
+      <c r="C19" t="s">
+        <v>410</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1a.1","Indicator":"No. of clients who received counseling and testing (CT) services for HIV and received their test results this month"},</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>384</v>
+      </c>
+      <c r="C20" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1b","Indicator":"Number of all clients who tested  HIV positive for HIV and collected test results."},</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>385</v>
+      </c>
+      <c r="C21" t="s">
+        <v>386</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1b.1","Indicator":"Number of clients who tested as couple and collected test results at this facility this month."},</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" t="s">
+        <v>388</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1c","Indicator":"Numbner of HIV DISCONDANT couples who received test results. (Count Females only)."},</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>389</v>
+      </c>
+      <c r="C23" t="s">
+        <v>390</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1c.1","Indicator":"Number of clients who were re-tested for HIV and received there results"},</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>391</v>
+      </c>
+      <c r="C24" t="s">
+        <v>392</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT1d","Indicator":"Number of clients who re-tested and tested positive for HIV."},</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25" t="s">
+        <v>414</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e","Indicator":"Numbner of clients who Tested for HIV through PITC (Total of PMTCT,STI,TB,MC,CECAP,FP)"},</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>394</v>
+      </c>
+      <c r="C26" t="s">
+        <v>395</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.1","Indicator":"Number of clients who tested for HIV through PMTCT"},</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>396</v>
+      </c>
+      <c r="C27" t="s">
+        <v>397</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.2","Indicator":"Number of clients who tested for HIV through TB"},</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>398</v>
+      </c>
+      <c r="C28" t="s">
+        <v>399</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.3","Indicator":"Number of clients who tested for HIV through STI"},</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>400</v>
+      </c>
+      <c r="C29" t="s">
+        <v>401</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.4","Indicator":"Number of clients who tested for HIV through FP"},</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>402</v>
+      </c>
+      <c r="C30" t="s">
+        <v>403</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.5","Indicator":"Number of clients who tested for HIV through CECAP"},</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C31" t="s">
+        <v>405</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.6","Indicator":"Number of clients who tested for HIV through VMMC"},</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>406</v>
+      </c>
+      <c r="C32" t="s">
+        <v>407</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.e.7","Indicator":"Number of Clients who tested positive from PITC"},</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>408</v>
+      </c>
+      <c r="C33" t="s">
+        <v>409</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IndicatorId":"CT.f","Indicator":"Total number of clients referred for Pre ART Care Services this Months"},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>